<commit_message>
atualizando a build + beta
</commit_message>
<xml_diff>
--- a/data/Ex1.xlsx
+++ b/data/Ex1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Element"/>
@@ -83,7 +83,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -433,7 +433,7 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -565,7 +565,7 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>